<commit_message>
Added code for adverse effect bar plot by severity
</commit_message>
<xml_diff>
--- a/data/effects_severity.xlsx
+++ b/data/effects_severity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Ciitizen-health-scn8a/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98033B5B-5605-AA42-8757-628AF847AA14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D9BC4F-B76D-584E-BAB7-FF982B46884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
   <si>
     <t>Increased seizure frequency</t>
   </si>
@@ -317,18 +317,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -630,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -982,6 +971,9 @@
       <c r="A47" t="s">
         <v>28</v>
       </c>
+      <c r="B47" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">

</xml_diff>

<commit_message>
Modified Figure 2D and adverse effects figures
</commit_message>
<xml_diff>
--- a/data/effects_severity.xlsx
+++ b/data/effects_severity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Ciitizen-health-scn8a/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D9BC4F-B76D-584E-BAB7-FF982B46884B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E32908-1994-1845-BFE6-96E76289BCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -737,8 +737,8 @@
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>69</v>
+      <c r="B14" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
merged local branch to main
</commit_message>
<xml_diff>
--- a/data/effects_severity.xlsx
+++ b/data/effects_severity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kiran/Documents/GitHub/Ciitizen-health-scn8a/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elysetanzer/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E32908-1994-1845-BFE6-96E76289BCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B64B44-4A1A-A440-A2EA-95FD7BEBE329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4340" yWindow="760" windowWidth="30220" windowHeight="20240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="70">
   <si>
     <t>Increased seizure frequency</t>
   </si>
@@ -619,8 +619,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="193" zoomScaleNormal="193" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="91" zoomScaleNormal="193" workbookViewId="0">
+      <selection activeCell="F64" sqref="F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -921,51 +921,81 @@
       <c r="A37" t="s">
         <v>4</v>
       </c>
+      <c r="B37" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>5</v>
       </c>
+      <c r="B38" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>7</v>
       </c>
+      <c r="B39" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>8</v>
       </c>
+      <c r="B40" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>13</v>
       </c>
+      <c r="B41" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>19</v>
       </c>
+      <c r="B42" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>21</v>
       </c>
+      <c r="B43" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>22</v>
       </c>
+      <c r="B44" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>25</v>
       </c>
+      <c r="B45" s="3" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>27</v>
       </c>
+      <c r="B46" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
@@ -979,95 +1009,152 @@
       <c r="A48" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B52" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B56" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B57" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B58" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B59" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B60" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B61" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B62" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B63" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B64" s="3" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>64</v>
+      </c>
+      <c r="B66" s="2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>